<commit_message>
Data for xG trendline
</commit_message>
<xml_diff>
--- a/Data/Chelsea_xG.xlsx
+++ b/Data/Chelsea_xG.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\anish\Documents\projects\Football-Analytics\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D287688B-A8C7-463C-9EF4-831C5E6A3818}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{205BE794-A47D-4480-9DF8-09B1FF433A2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2730" yWindow="2730" windowWidth="21600" windowHeight="11295" xr2:uid="{EE63B618-CBFC-48C6-88DE-C608A450462E}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="310" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="424" uniqueCount="35">
   <si>
     <t>Round</t>
   </si>
@@ -122,6 +122,15 @@
   </si>
   <si>
     <t>Season</t>
+  </si>
+  <si>
+    <t>21/22</t>
+  </si>
+  <si>
+    <t>20/21</t>
+  </si>
+  <si>
+    <t>19/20</t>
   </si>
 </sst>
 </file>
@@ -498,8 +507,8 @@
   <dimension ref="A1:F115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A97" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C116" sqref="C116"/>
+      <pane ySplit="1" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M40" sqref="M40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -547,8 +556,8 @@
       <c r="E2">
         <v>2.2999999999999998</v>
       </c>
-      <c r="F2">
-        <v>1</v>
+      <c r="F2" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -567,8 +576,8 @@
       <c r="E3">
         <v>0.8</v>
       </c>
-      <c r="F3">
-        <v>1</v>
+      <c r="F3" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -587,8 +596,8 @@
       <c r="E4">
         <v>1.2</v>
       </c>
-      <c r="F4">
-        <v>1</v>
+      <c r="F4" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -607,8 +616,8 @@
       <c r="E5">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F5">
-        <v>1</v>
+      <c r="F5" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -627,8 +636,8 @@
       <c r="E6">
         <v>1.6</v>
       </c>
-      <c r="F6">
-        <v>1</v>
+      <c r="F6" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -647,8 +656,8 @@
       <c r="E7">
         <v>0.9</v>
       </c>
-      <c r="F7">
-        <v>1</v>
+      <c r="F7" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -667,8 +676,8 @@
       <c r="E8">
         <v>0.5</v>
       </c>
-      <c r="F8">
-        <v>1</v>
+      <c r="F8" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -687,8 +696,8 @@
       <c r="E9">
         <v>1</v>
       </c>
-      <c r="F9">
-        <v>1</v>
+      <c r="F9" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -707,8 +716,8 @@
       <c r="E10">
         <v>0.3</v>
       </c>
-      <c r="F10">
-        <v>1</v>
+      <c r="F10" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -727,8 +736,8 @@
       <c r="E11">
         <v>2.2000000000000002</v>
       </c>
-      <c r="F11">
-        <v>1</v>
+      <c r="F11" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -747,8 +756,8 @@
       <c r="E12">
         <v>1.4</v>
       </c>
-      <c r="F12">
-        <v>1</v>
+      <c r="F12" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -767,8 +776,8 @@
       <c r="E13">
         <v>0.2</v>
       </c>
-      <c r="F13">
-        <v>1</v>
+      <c r="F13" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -787,8 +796,8 @@
       <c r="E14">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F14">
-        <v>1</v>
+      <c r="F14" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -807,8 +816,8 @@
       <c r="E15">
         <v>0.8</v>
       </c>
-      <c r="F15">
-        <v>1</v>
+      <c r="F15" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -827,8 +836,8 @@
       <c r="E16">
         <v>0.7</v>
       </c>
-      <c r="F16">
-        <v>1</v>
+      <c r="F16" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.25">
@@ -847,8 +856,8 @@
       <c r="E17">
         <v>1.7</v>
       </c>
-      <c r="F17">
-        <v>1</v>
+      <c r="F17" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.25">
@@ -867,8 +876,8 @@
       <c r="E18">
         <v>0.8</v>
       </c>
-      <c r="F18">
-        <v>1</v>
+      <c r="F18" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.25">
@@ -887,8 +896,8 @@
       <c r="E19">
         <v>0.4</v>
       </c>
-      <c r="F19">
-        <v>1</v>
+      <c r="F19" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.25">
@@ -907,8 +916,8 @@
       <c r="E20">
         <v>0.7</v>
       </c>
-      <c r="F20">
-        <v>1</v>
+      <c r="F20" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
@@ -927,8 +936,8 @@
       <c r="E21">
         <v>0.8</v>
       </c>
-      <c r="F21">
-        <v>1</v>
+      <c r="F21" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.25">
@@ -947,8 +956,8 @@
       <c r="E22">
         <v>0.9</v>
       </c>
-      <c r="F22">
-        <v>1</v>
+      <c r="F22" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.25">
@@ -967,8 +976,8 @@
       <c r="E23">
         <v>0.4</v>
       </c>
-      <c r="F23">
-        <v>1</v>
+      <c r="F23" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.25">
@@ -987,8 +996,8 @@
       <c r="E24">
         <v>0.6</v>
       </c>
-      <c r="F24">
-        <v>1</v>
+      <c r="F24" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.25">
@@ -1007,8 +1016,8 @@
       <c r="E25">
         <v>0.5</v>
       </c>
-      <c r="F25">
-        <v>1</v>
+      <c r="F25" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.25">
@@ -1027,8 +1036,8 @@
       <c r="E26">
         <v>1.6</v>
       </c>
-      <c r="F26">
-        <v>1</v>
+      <c r="F26" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.25">
@@ -1047,8 +1056,8 @@
       <c r="E27">
         <v>0.8</v>
       </c>
-      <c r="F27">
-        <v>1</v>
+      <c r="F27" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.25">
@@ -1067,8 +1076,8 @@
       <c r="E28">
         <v>0.4</v>
       </c>
-      <c r="F28">
-        <v>1</v>
+      <c r="F28" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.25">
@@ -1087,8 +1096,8 @@
       <c r="E29">
         <v>1.9</v>
       </c>
-      <c r="F29">
-        <v>1</v>
+      <c r="F29" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.25">
@@ -1107,8 +1116,8 @@
       <c r="E30">
         <v>0.6</v>
       </c>
-      <c r="F30">
-        <v>1</v>
+      <c r="F30" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.25">
@@ -1127,8 +1136,8 @@
       <c r="E31">
         <v>1.1000000000000001</v>
       </c>
-      <c r="F31">
-        <v>1</v>
+      <c r="F31" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.25">
@@ -1147,8 +1156,8 @@
       <c r="E32">
         <v>0.5</v>
       </c>
-      <c r="F32">
-        <v>1</v>
+      <c r="F32" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.25">
@@ -1167,8 +1176,8 @@
       <c r="E33">
         <v>2.8</v>
       </c>
-      <c r="F33">
-        <v>1</v>
+      <c r="F33" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.25">
@@ -1187,8 +1196,8 @@
       <c r="E34">
         <v>0.4</v>
       </c>
-      <c r="F34">
-        <v>1</v>
+      <c r="F34" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.25">
@@ -1207,8 +1216,8 @@
       <c r="E35">
         <v>1.4</v>
       </c>
-      <c r="F35">
-        <v>1</v>
+      <c r="F35" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.25">
@@ -1227,8 +1236,8 @@
       <c r="E36">
         <v>1.9</v>
       </c>
-      <c r="F36">
-        <v>1</v>
+      <c r="F36" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.25">
@@ -1247,8 +1256,8 @@
       <c r="E37">
         <v>0</v>
       </c>
-      <c r="F37">
-        <v>1</v>
+      <c r="F37" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.25">
@@ -1267,8 +1276,8 @@
       <c r="E38">
         <v>1.4</v>
       </c>
-      <c r="F38">
-        <v>1</v>
+      <c r="F38" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.25">
@@ -1287,8 +1296,8 @@
       <c r="E39">
         <v>0.2</v>
       </c>
-      <c r="F39">
-        <v>1</v>
+      <c r="F39" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.25">
@@ -1307,8 +1316,8 @@
       <c r="E40">
         <v>1.4</v>
       </c>
-      <c r="F40">
-        <v>2</v>
+      <c r="F40" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
@@ -1327,8 +1336,8 @@
       <c r="E41">
         <v>2.6</v>
       </c>
-      <c r="F41">
-        <v>2</v>
+      <c r="F41" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
@@ -1347,8 +1356,8 @@
       <c r="E42">
         <v>1</v>
       </c>
-      <c r="F42">
-        <v>2</v>
+      <c r="F42" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
@@ -1367,8 +1376,8 @@
       <c r="E43">
         <v>0.1</v>
       </c>
-      <c r="F43">
-        <v>2</v>
+      <c r="F43" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.25">
@@ -1387,8 +1396,8 @@
       <c r="E44">
         <v>2.2000000000000002</v>
       </c>
-      <c r="F44">
-        <v>2</v>
+      <c r="F44" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.25">
@@ -1407,8 +1416,8 @@
       <c r="E45">
         <v>0.7</v>
       </c>
-      <c r="F45">
-        <v>2</v>
+      <c r="F45" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.25">
@@ -1427,8 +1436,8 @@
       <c r="E46">
         <v>0.4</v>
       </c>
-      <c r="F46">
-        <v>2</v>
+      <c r="F46" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.25">
@@ -1447,8 +1456,8 @@
       <c r="E47">
         <v>0.6</v>
       </c>
-      <c r="F47">
-        <v>2</v>
+      <c r="F47" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.25">
@@ -1467,8 +1476,8 @@
       <c r="E48">
         <v>0.6</v>
       </c>
-      <c r="F48">
-        <v>2</v>
+      <c r="F48" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.25">
@@ -1487,8 +1496,8 @@
       <c r="E49">
         <v>0.2</v>
       </c>
-      <c r="F49">
-        <v>2</v>
+      <c r="F49" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.25">
@@ -1507,8 +1516,8 @@
       <c r="E50">
         <v>1.3</v>
       </c>
-      <c r="F50">
-        <v>2</v>
+      <c r="F50" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.25">
@@ -1527,8 +1536,8 @@
       <c r="E51">
         <v>1.3</v>
       </c>
-      <c r="F51">
-        <v>2</v>
+      <c r="F51" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.25">
@@ -1547,8 +1556,8 @@
       <c r="E52">
         <v>0.5</v>
       </c>
-      <c r="F52">
-        <v>2</v>
+      <c r="F52" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.25">
@@ -1567,8 +1576,8 @@
       <c r="E53">
         <v>0.5</v>
       </c>
-      <c r="F53">
-        <v>2</v>
+      <c r="F53" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.25">
@@ -1587,8 +1596,8 @@
       <c r="E54">
         <v>2.1</v>
       </c>
-      <c r="F54">
-        <v>2</v>
+      <c r="F54" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.25">
@@ -1607,8 +1616,8 @@
       <c r="E55">
         <v>0.8</v>
       </c>
-      <c r="F55">
-        <v>2</v>
+      <c r="F55" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.25">
@@ -1627,8 +1636,8 @@
       <c r="E56">
         <v>2.4</v>
       </c>
-      <c r="F56">
-        <v>2</v>
+      <c r="F56" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.25">
@@ -1647,8 +1656,8 @@
       <c r="E57">
         <v>0.8</v>
       </c>
-      <c r="F57">
-        <v>2</v>
+      <c r="F57" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.25">
@@ -1667,8 +1676,8 @@
       <c r="E58">
         <v>1.2</v>
       </c>
-      <c r="F58">
-        <v>2</v>
+      <c r="F58" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.25">
@@ -1687,8 +1696,8 @@
       <c r="E59">
         <v>0.4</v>
       </c>
-      <c r="F59">
-        <v>2</v>
+      <c r="F59" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.25">
@@ -1707,8 +1716,8 @@
       <c r="E60">
         <v>0.2</v>
       </c>
-      <c r="F60">
-        <v>2</v>
+      <c r="F60" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.25">
@@ -1727,8 +1736,8 @@
       <c r="E61">
         <v>0.3</v>
       </c>
-      <c r="F61">
-        <v>2</v>
+      <c r="F61" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.25">
@@ -1747,8 +1756,8 @@
       <c r="E62">
         <v>0.4</v>
       </c>
-      <c r="F62">
-        <v>2</v>
+      <c r="F62" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.25">
@@ -1767,8 +1776,8 @@
       <c r="E63">
         <v>0.7</v>
       </c>
-      <c r="F63">
-        <v>2</v>
+      <c r="F63" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.25">
@@ -1787,8 +1796,8 @@
       <c r="E64">
         <v>0.5</v>
       </c>
-      <c r="F64">
-        <v>2</v>
+      <c r="F64" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
@@ -1807,8 +1816,8 @@
       <c r="E65">
         <v>0.5</v>
       </c>
-      <c r="F65">
-        <v>2</v>
+      <c r="F65" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.25">
@@ -1827,8 +1836,8 @@
       <c r="E66">
         <v>0.3</v>
       </c>
-      <c r="F66">
-        <v>2</v>
+      <c r="F66" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.25">
@@ -1847,8 +1856,8 @@
       <c r="E67">
         <v>0.3</v>
       </c>
-      <c r="F67">
-        <v>2</v>
+      <c r="F67" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
@@ -1867,8 +1876,8 @@
       <c r="E68">
         <v>0.4</v>
       </c>
-      <c r="F68">
-        <v>2</v>
+      <c r="F68" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.25">
@@ -1887,8 +1896,8 @@
       <c r="E69">
         <v>1.9</v>
       </c>
-      <c r="F69">
-        <v>2</v>
+      <c r="F69" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
@@ -1907,8 +1916,8 @@
       <c r="E70">
         <v>0.1</v>
       </c>
-      <c r="F70">
-        <v>2</v>
+      <c r="F70" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
@@ -1927,8 +1936,8 @@
       <c r="E71">
         <v>0.7</v>
       </c>
-      <c r="F71">
-        <v>2</v>
+      <c r="F71" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
@@ -1947,8 +1956,8 @@
       <c r="E72">
         <v>0.4</v>
       </c>
-      <c r="F72">
-        <v>2</v>
+      <c r="F72" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.25">
@@ -1967,8 +1976,8 @@
       <c r="E73">
         <v>0.3</v>
       </c>
-      <c r="F73">
-        <v>2</v>
+      <c r="F73" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.25">
@@ -1987,8 +1996,8 @@
       <c r="E74">
         <v>2.2000000000000002</v>
       </c>
-      <c r="F74">
-        <v>2</v>
+      <c r="F74" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.25">
@@ -2007,8 +2016,8 @@
       <c r="E75">
         <v>0.8</v>
       </c>
-      <c r="F75">
-        <v>2</v>
+      <c r="F75" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.25">
@@ -2027,8 +2036,8 @@
       <c r="E76">
         <v>0.9</v>
       </c>
-      <c r="F76">
-        <v>2</v>
+      <c r="F76" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
@@ -2047,8 +2056,8 @@
       <c r="E77">
         <v>1</v>
       </c>
-      <c r="F77">
-        <v>2</v>
+      <c r="F77" t="s">
+        <v>33</v>
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
@@ -2067,8 +2076,8 @@
       <c r="E78">
         <v>0.3</v>
       </c>
-      <c r="F78">
-        <v>3</v>
+      <c r="F78" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
@@ -2087,8 +2096,8 @@
       <c r="E79">
         <v>0.3</v>
       </c>
-      <c r="F79">
-        <v>3</v>
+      <c r="F79" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
@@ -2107,8 +2116,8 @@
       <c r="E80">
         <v>2.6</v>
       </c>
-      <c r="F80">
-        <v>3</v>
+      <c r="F80" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
@@ -2127,8 +2136,8 @@
       <c r="E81">
         <v>1.5</v>
       </c>
-      <c r="F81">
-        <v>3</v>
+      <c r="F81" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
@@ -2147,8 +2156,8 @@
       <c r="E82">
         <v>0.7</v>
       </c>
-      <c r="F82">
-        <v>3</v>
+      <c r="F82" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
@@ -2167,8 +2176,8 @@
       <c r="E83">
         <v>1.7</v>
       </c>
-      <c r="F83">
-        <v>3</v>
+      <c r="F83" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
@@ -2187,8 +2196,8 @@
       <c r="E84">
         <v>1.3</v>
       </c>
-      <c r="F84">
-        <v>3</v>
+      <c r="F84" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
@@ -2207,8 +2216,8 @@
       <c r="E85">
         <v>1.6</v>
       </c>
-      <c r="F85">
-        <v>3</v>
+      <c r="F85" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
@@ -2227,8 +2236,8 @@
       <c r="E86">
         <v>0.2</v>
       </c>
-      <c r="F86">
-        <v>3</v>
+      <c r="F86" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
@@ -2247,8 +2256,8 @@
       <c r="E87">
         <v>0.3</v>
       </c>
-      <c r="F87">
-        <v>3</v>
+      <c r="F87" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
@@ -2267,8 +2276,8 @@
       <c r="E88">
         <v>1</v>
       </c>
-      <c r="F88">
-        <v>3</v>
+      <c r="F88" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
@@ -2287,8 +2296,8 @@
       <c r="E89">
         <v>0.4</v>
       </c>
-      <c r="F89">
-        <v>3</v>
+      <c r="F89" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
@@ -2307,8 +2316,8 @@
       <c r="E90">
         <v>0.7</v>
       </c>
-      <c r="F90">
-        <v>3</v>
+      <c r="F90" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
@@ -2327,8 +2336,8 @@
       <c r="E91">
         <v>1</v>
       </c>
-      <c r="F91">
-        <v>3</v>
+      <c r="F91" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
@@ -2347,8 +2356,8 @@
       <c r="E92">
         <v>1.8</v>
       </c>
-      <c r="F92">
-        <v>3</v>
+      <c r="F92" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
@@ -2367,8 +2376,8 @@
       <c r="E93">
         <v>1.4</v>
       </c>
-      <c r="F93">
-        <v>3</v>
+      <c r="F93" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
@@ -2387,8 +2396,8 @@
       <c r="E94">
         <v>0.4</v>
       </c>
-      <c r="F94">
-        <v>3</v>
+      <c r="F94" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
@@ -2407,8 +2416,8 @@
       <c r="E95">
         <v>0.3</v>
       </c>
-      <c r="F95">
-        <v>3</v>
+      <c r="F95" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
@@ -2427,8 +2436,8 @@
       <c r="E96">
         <v>0.6</v>
       </c>
-      <c r="F96">
-        <v>3</v>
+      <c r="F96" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
@@ -2447,8 +2456,8 @@
       <c r="E97">
         <v>0.9</v>
       </c>
-      <c r="F97">
-        <v>3</v>
+      <c r="F97" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
@@ -2467,8 +2476,8 @@
       <c r="E98">
         <v>1.4</v>
       </c>
-      <c r="F98">
-        <v>3</v>
+      <c r="F98" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
@@ -2487,8 +2496,8 @@
       <c r="E99">
         <v>0.7</v>
       </c>
-      <c r="F99">
-        <v>3</v>
+      <c r="F99" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
@@ -2507,8 +2516,8 @@
       <c r="E100">
         <v>0.6</v>
       </c>
-      <c r="F100">
-        <v>3</v>
+      <c r="F100" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
@@ -2527,8 +2536,8 @@
       <c r="E101">
         <v>0.4</v>
       </c>
-      <c r="F101">
-        <v>3</v>
+      <c r="F101" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
@@ -2547,8 +2556,8 @@
       <c r="E102">
         <v>0.6</v>
       </c>
-      <c r="F102">
-        <v>3</v>
+      <c r="F102" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
@@ -2567,8 +2576,8 @@
       <c r="E103">
         <v>0.8</v>
       </c>
-      <c r="F103">
-        <v>3</v>
+      <c r="F103" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
@@ -2587,8 +2596,8 @@
       <c r="E104">
         <v>1</v>
       </c>
-      <c r="F104">
-        <v>3</v>
+      <c r="F104" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
@@ -2607,8 +2616,8 @@
       <c r="E105">
         <v>0.2</v>
       </c>
-      <c r="F105">
-        <v>3</v>
+      <c r="F105" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
@@ -2627,8 +2636,8 @@
       <c r="E106">
         <v>2.1</v>
       </c>
-      <c r="F106">
-        <v>3</v>
+      <c r="F106" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
@@ -2647,8 +2656,8 @@
       <c r="E107">
         <v>0.5</v>
       </c>
-      <c r="F107">
-        <v>3</v>
+      <c r="F107" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
@@ -2667,8 +2676,8 @@
       <c r="E108">
         <v>2.4</v>
       </c>
-      <c r="F108">
-        <v>3</v>
+      <c r="F108" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
@@ -2687,8 +2696,8 @@
       <c r="E109">
         <v>0.5</v>
       </c>
-      <c r="F109">
-        <v>3</v>
+      <c r="F109" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
@@ -2707,8 +2716,8 @@
       <c r="E110">
         <v>0.6</v>
       </c>
-      <c r="F110">
-        <v>3</v>
+      <c r="F110" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
@@ -2727,8 +2736,8 @@
       <c r="E111">
         <v>1.3</v>
       </c>
-      <c r="F111">
-        <v>3</v>
+      <c r="F111" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
@@ -2747,8 +2756,8 @@
       <c r="E112">
         <v>2.1</v>
       </c>
-      <c r="F112">
-        <v>3</v>
+      <c r="F112" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
@@ -2767,8 +2776,8 @@
       <c r="E113">
         <v>0.5</v>
       </c>
-      <c r="F113">
-        <v>3</v>
+      <c r="F113" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
@@ -2787,8 +2796,8 @@
       <c r="E114">
         <v>0.1</v>
       </c>
-      <c r="F114">
-        <v>3</v>
+      <c r="F114" t="s">
+        <v>32</v>
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
@@ -2807,8 +2816,8 @@
       <c r="E115">
         <v>1</v>
       </c>
-      <c r="F115">
-        <v>3</v>
+      <c r="F115" t="s">
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>